<commit_message>
Integrate new euro conversion factors for web-app/OCCF
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Documents\eps-us\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0104BD1-7907-4774-8B4A-D77E893CD0A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="45" windowWidth="23955" windowHeight="11325"/>
+    <workbookView xWindow="38400" yWindow="3855" windowWidth="18420" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -17,12 +18,23 @@
     <sheet name="OCCF-DpMOCU" sheetId="4" r:id="rId3"/>
     <sheet name="OCCF-DpSOCU" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913" iterate="1" iterateDelta="1.0000000000000001E-5"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Source:</t>
   </si>
@@ -54,9 +66,6 @@
     <t>One Large Output Currency Unit</t>
   </si>
   <si>
-    <t>For the U.S. model:</t>
-  </si>
-  <si>
     <t>Large Output Currency Unit</t>
   </si>
   <si>
@@ -72,18 +81,21 @@
     <t>OCCF Dollars per Small Output Currency Unit</t>
   </si>
   <si>
-    <t>2018 dollars</t>
-  </si>
-  <si>
     <t>See cpi.xlsx</t>
   </si>
   <si>
+    <t>which in this case is "2012 dollars per 2018 dollar."</t>
+  </si>
+  <si>
     <t>2012 dollars are worth more than 2018 dollars, so we need a</t>
   </si>
   <si>
     <t>value less than 1 in this variable.</t>
   </si>
   <si>
+    <t>2018 dollars per 2012 dollar</t>
+  </si>
+  <si>
     <t>This is why we multiply, not divide, by the conversion</t>
   </si>
   <si>
@@ -99,23 +111,35 @@
     <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
   </si>
   <si>
-    <t>2019 dollars per 2012 dollar</t>
-  </si>
-  <si>
-    <t>which in this case is "2012 dollars per 2019 dollar."</t>
-  </si>
-  <si>
-    <t>million 2019 dollars</t>
-  </si>
-  <si>
-    <t>billion 2019 dollars</t>
+    <t>For the EU model:</t>
+  </si>
+  <si>
+    <t>billion 2018 euro</t>
+  </si>
+  <si>
+    <t>million 2018 euro</t>
+  </si>
+  <si>
+    <t>2018 euro</t>
+  </si>
+  <si>
+    <t>2018 euro per 2018 dollar</t>
+  </si>
+  <si>
+    <t>2018 euro per 2012 dollar</t>
+  </si>
+  <si>
+    <t>https://www.exchangerates.org.uk/USD-EUR-spot-exchange-rates-history-2018.html</t>
+  </si>
+  <si>
+    <t>2018 euro conversion</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="28" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -131,8 +155,195 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="6"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color indexed="30"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +356,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -154,11 +538,326 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color theme="4"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="dashed">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color theme="0"/>
+      </left>
+      <right style="thick">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF0096D7"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dashed">
+        <color rgb="FFBFBFBF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF0096D7"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" applyNumberFormat="0" applyFont="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="15" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFont="0" applyFill="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFont="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyProtection="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyProtection="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -170,12 +869,121 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="43" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="77">
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1 2" xfId="62" xr:uid="{29DBD619-DD33-4689-AB6A-0726714D6FC9}"/>
+    <cellStyle name="20% - Accent2" xfId="21" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2 2" xfId="64" xr:uid="{731CD6AC-29B1-42BC-B047-D5894578FA15}"/>
+    <cellStyle name="20% - Accent3" xfId="24" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3 2" xfId="66" xr:uid="{EE8939B5-F3F2-45A8-8F2F-547F073D8B41}"/>
+    <cellStyle name="20% - Accent4" xfId="27" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4 2" xfId="68" xr:uid="{0C931584-31B0-4AB1-AFC9-958C1754A32B}"/>
+    <cellStyle name="20% - Accent5" xfId="30" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5 2" xfId="70" xr:uid="{99FB16E0-E479-4E49-BB38-4CE00F5F87EB}"/>
+    <cellStyle name="20% - Accent6" xfId="33" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6 2" xfId="72" xr:uid="{E84EEEDF-6E7D-4261-9718-F9D88E2CFCF7}"/>
+    <cellStyle name="40% - Accent1" xfId="19" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1 2" xfId="63" xr:uid="{871E8807-EE4B-47D8-92AD-AC7FB4D8BD8A}"/>
+    <cellStyle name="40% - Accent2" xfId="22" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2 2" xfId="65" xr:uid="{584EDF94-7BA3-4C29-9DFA-D48BF2554F9F}"/>
+    <cellStyle name="40% - Accent3" xfId="25" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3 2" xfId="67" xr:uid="{9EF65AA7-B078-40EF-BE2D-C8C6C1273598}"/>
+    <cellStyle name="40% - Accent4" xfId="28" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4 2" xfId="69" xr:uid="{E6A51E7D-4346-4B58-8383-EA0173C7A77F}"/>
+    <cellStyle name="40% - Accent5" xfId="31" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5 2" xfId="71" xr:uid="{5486E4D5-9A1E-418B-A5AE-D97366826154}"/>
+    <cellStyle name="40% - Accent6" xfId="34" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6 2" xfId="73" xr:uid="{AC7C56BE-B4EB-4FF5-9182-56E402F56690}"/>
+    <cellStyle name="60% - Accent1 2" xfId="55" xr:uid="{F5D1A643-567E-43F2-86BC-5F1F74825AB2}"/>
+    <cellStyle name="60% - Accent2 2" xfId="56" xr:uid="{C7BBB4FF-493E-49D6-92D3-2A1F36F806EF}"/>
+    <cellStyle name="60% - Accent3 2" xfId="57" xr:uid="{3E7C0407-7B17-4F98-A1CF-775025EBCB68}"/>
+    <cellStyle name="60% - Accent4 2" xfId="58" xr:uid="{4D79FFFD-76D5-4496-98A7-4FCFD4EFE4B7}"/>
+    <cellStyle name="60% - Accent5 2" xfId="59" xr:uid="{CBD67ED6-EF14-4ED1-AE36-84F58C2D4F0C}"/>
+    <cellStyle name="60% - Accent6 2" xfId="60" xr:uid="{AA656FCB-BF3A-462E-95F6-DED5286A1D0C}"/>
+    <cellStyle name="Accent1" xfId="17" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="20" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="23" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="26" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="29" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="32" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Body: normal cell" xfId="36" xr:uid="{AAE7F109-DF07-4DB5-8927-38E5292EC090}"/>
+    <cellStyle name="Body: normal cell 2" xfId="49" xr:uid="{774AF1E4-6618-4D3C-B543-5A8510FAF47E}"/>
+    <cellStyle name="Calculation" xfId="10" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="12" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="15" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" customBuiltin="1"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="42" xr:uid="{81D6EC52-49BA-44E2-BC74-836BA7E30212}"/>
+    <cellStyle name="Font: Calibri, 9pt regular 2" xfId="52" xr:uid="{64DD6255-4EB8-4557-AB27-44AD85BF6379}"/>
+    <cellStyle name="Footnotes: all except top row" xfId="45" xr:uid="{49AFDA6E-87AF-4E22-AF24-4BB9B51D5D4B}"/>
+    <cellStyle name="Footnotes: top row" xfId="40" xr:uid="{58D85F0C-F688-43F1-9867-04EE3BCFB2E1}"/>
+    <cellStyle name="Footnotes: top row 2" xfId="48" xr:uid="{9E6183CA-5244-4C8D-9C03-6D4A8690CF6A}"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Header: bottom row" xfId="35" xr:uid="{ACA4C717-567D-412B-B7F2-88A14AAF58DD}"/>
+    <cellStyle name="Header: bottom row 2" xfId="51" xr:uid="{F44096B2-FD75-48EB-B31F-D8CFC04710C5}"/>
+    <cellStyle name="Header: top rows" xfId="37" xr:uid="{76212F36-7E87-429B-AA4F-A9F063A906EC}"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="8" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral 2" xfId="54" xr:uid="{0C97473C-AF50-47A4-AD7E-BFB6A8D6FE13}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="47" xr:uid="{6C9FE47E-08D5-45F2-8581-237D50F68423}"/>
+    <cellStyle name="Normal 3" xfId="75" xr:uid="{8E2C68E3-3940-41D2-947C-9C4AD210277C}"/>
+    <cellStyle name="Note" xfId="14" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note 2" xfId="61" xr:uid="{87F4DF08-56F9-4172-BAD0-E1E8DF233549}"/>
+    <cellStyle name="Output" xfId="9" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Parent row" xfId="39" xr:uid="{FF12012D-6416-4E3C-AE42-DDF964BE396E}"/>
+    <cellStyle name="Parent row 2" xfId="50" xr:uid="{7F2F950A-8699-4064-A7D3-F705F6891BA8}"/>
+    <cellStyle name="Percent 2" xfId="76" xr:uid="{06BC8F68-460A-4BBA-BF10-B0184222F838}"/>
+    <cellStyle name="Section Break" xfId="41" xr:uid="{A3200D91-7BC0-453E-B025-EBD93FE595CC}"/>
+    <cellStyle name="Section Break: parent row" xfId="38" xr:uid="{E0CA4011-0D71-4329-8D6B-F31FEE02BB01}"/>
+    <cellStyle name="Standard 2" xfId="74" xr:uid="{ED0FDB6D-ABF5-4A86-8FA4-B7D3E05444BD}"/>
+    <cellStyle name="Table title" xfId="46" xr:uid="{D3504562-4E0D-4D4F-9BB1-2544C77E63B7}"/>
+    <cellStyle name="Table title 2" xfId="53" xr:uid="{D638445B-22E4-4A11-AA65-3F2A353D1A6D}"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="16" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="13" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom style="thick">
+          <color theme="4"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical/>
+        <horizontal style="dotted">
+          <color theme="0" tint="-0.24994659260841701"/>
+        </horizontal>
+      </border>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Table Style 1" pivot="0" count="2" xr9:uid="{D7C69608-5F4E-4AF9-AF65-34E48B98EF23}">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -263,6 +1071,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -298,6 +1123,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -473,11 +1315,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -487,7 +1329,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
@@ -497,7 +1339,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -505,128 +1347,194 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B8" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" s="1" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>6</v>
+      <c r="A12" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A17" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="6"/>
-    </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>28</v>
+      <c r="A18" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="B20" s="6"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A26">
-        <v>0.89805481563188172</v>
-      </c>
-      <c r="B26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B28" t="s">
-        <v>24</v>
+      <c r="A26" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="6"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A27" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A29" s="10">
+        <v>0.84750000000000003</v>
+      </c>
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B30" t="s">
-        <v>18</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A30" s="9">
+        <v>0.9143273584567535</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A31">
+        <f>A29*A30</f>
+        <v>0.77489243629209859</v>
+      </c>
       <c r="B31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B32" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B33" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B34" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B36" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
+      <c r="B38" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B8" r:id="rId1" xr:uid="{71546DD5-F32F-4B71-ADDD-6A129D24A1CC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="31.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
+        <f>10^9*About!$A$31</f>
+        <v>774892436.29209864</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -641,16 +1549,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3">
-        <f>10^9*About!$A$26</f>
-        <v>898054815.63188171</v>
+      <c r="B2" s="8">
+        <f>10^6*About!$A$31</f>
+        <v>774892.4362920986</v>
       </c>
     </row>
   </sheetData>
@@ -658,8 +1566,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -674,49 +1582,16 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B1" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8">
-        <f>10^6*About!$A$26</f>
-        <v>898054.81563188171</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="B1" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="B2" s="7">
-        <f>1*About!A26</f>
-        <v>0.89805481563188172</v>
+        <f>1*About!A31</f>
+        <v>0.77489243629209859</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated EU web-app/OCCF files from 2018 to 2019 euros
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdeng\Dropbox (Energy Innovation)\EU EPS\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0104BD1-7907-4774-8B4A-D77E893CD0A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531DEFF4-07F2-4680-A219-042D558E7D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="3855" windowWidth="18420" windowHeight="15300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -84,18 +84,9 @@
     <t>See cpi.xlsx</t>
   </si>
   <si>
-    <t>which in this case is "2012 dollars per 2018 dollar."</t>
-  </si>
-  <si>
-    <t>2012 dollars are worth more than 2018 dollars, so we need a</t>
-  </si>
-  <si>
     <t>value less than 1 in this variable.</t>
   </si>
   <si>
-    <t>2018 dollars per 2012 dollar</t>
-  </si>
-  <si>
     <t>This is why we multiply, not divide, by the conversion</t>
   </si>
   <si>
@@ -114,25 +105,34 @@
     <t>For the EU model:</t>
   </si>
   <si>
-    <t>billion 2018 euro</t>
-  </si>
-  <si>
-    <t>million 2018 euro</t>
-  </si>
-  <si>
-    <t>2018 euro</t>
-  </si>
-  <si>
-    <t>2018 euro per 2018 dollar</t>
-  </si>
-  <si>
-    <t>2018 euro per 2012 dollar</t>
-  </si>
-  <si>
-    <t>https://www.exchangerates.org.uk/USD-EUR-spot-exchange-rates-history-2018.html</t>
-  </si>
-  <si>
-    <t>2018 euro conversion</t>
+    <t>https://www.exchangerates.org.uk/USD-EUR-spot-exchange-rates-history-2019.html</t>
+  </si>
+  <si>
+    <t>2019 euro conversion</t>
+  </si>
+  <si>
+    <t>billion 2019 euro</t>
+  </si>
+  <si>
+    <t>million 2019 euro</t>
+  </si>
+  <si>
+    <t>2019 euro</t>
+  </si>
+  <si>
+    <t>2019 euro per 2019 dollar</t>
+  </si>
+  <si>
+    <t>2019 dollars per 2012 dollar</t>
+  </si>
+  <si>
+    <t>2019 euro per 2012 dollar</t>
+  </si>
+  <si>
+    <t>which in this case is "2012 dollars per 2019 dollar."</t>
+  </si>
+  <si>
+    <t>2012 dollars are worth more than 2019 dollars, so we need a</t>
   </si>
 </sst>
 </file>
@@ -1319,30 +1319,30 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="26.265625" customWidth="1"/>
+    <col min="2" max="2" width="26.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,143 +1350,143 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
       <c r="B8" s="11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75"/>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A12" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A18" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A23" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="6"/>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A24" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A26" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B26" s="6"/>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="A29" s="10">
+        <v>0.89290000000000003</v>
+      </c>
+      <c r="B29" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A29" s="10">
-        <v>0.84750000000000003</v>
-      </c>
-      <c r="B29" t="s">
+    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
+      <c r="A30" s="9">
+        <v>0.89805000000000001</v>
+      </c>
+      <c r="B30" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="9">
-        <v>0.9143273584567535</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A31">
         <f>A29*A30</f>
-        <v>0.77489243629209859</v>
+        <v>0.801868845</v>
       </c>
       <c r="B31" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.75">
       <c r="B33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.75">
       <c r="B34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.75">
+      <c r="B35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.75">
+      <c r="B36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B35" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.75">
+      <c r="B37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B36" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.75">
+      <c r="B38" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.45">
-      <c r="B38" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1509,23 +1509,23 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="3">
         <f>10^9*About!$A$31</f>
-        <v>774892436.29209864</v>
+        <v>801868845</v>
       </c>
     </row>
   </sheetData>
@@ -1542,23 +1542,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="8">
         <f>10^6*About!$A$31</f>
-        <v>774892.4362920986</v>
+        <v>801868.84499999997</v>
       </c>
     </row>
   </sheetData>
@@ -1575,23 +1575,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <cols>
-    <col min="2" max="2" width="31.265625" customWidth="1"/>
+    <col min="2" max="2" width="31.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="B1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="7">
         <f>1*About!A31</f>
-        <v>0.77489243629209859</v>
+        <v>0.801868845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Port input-data updates from eps-eu-ci (through commit 1e366cc) to align modeling
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\swenzel\Dropbox (Energy Innovation)\My PC (energy044)\Documents\GitHub_Repositories\eps-eu\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dobrien\Dropbox (Energy Innovation)\Desktop\Models\E.U. Models\eps-eu-ci\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{531DEFF4-07F2-4680-A219-042D558E7D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE361DF8-330D-4A3F-B139-884043994335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12600" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30495" yWindow="2130" windowWidth="27075" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t>Source:</t>
   </si>
@@ -120,19 +120,37 @@
     <t>2019 euro</t>
   </si>
   <si>
-    <t>2019 euro per 2019 dollar</t>
-  </si>
-  <si>
-    <t>2019 dollars per 2012 dollar</t>
-  </si>
-  <si>
-    <t>2019 euro per 2012 dollar</t>
-  </si>
-  <si>
     <t>which in this case is "2012 dollars per 2019 dollar."</t>
   </si>
   <si>
     <t>2012 dollars are worth more than 2019 dollars, so we need a</t>
+  </si>
+  <si>
+    <t>want</t>
+  </si>
+  <si>
+    <t>USD2012/EUR2019</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>USD2012/USD2019 * USD2019/EUR2019</t>
+  </si>
+  <si>
+    <t>USD2012 per EUR2019</t>
+  </si>
+  <si>
+    <t>USD2012 per USD2019</t>
+  </si>
+  <si>
+    <t>USD2019 per EUR2019</t>
+  </si>
+  <si>
+    <t>1 USD2019 = 0.8929 EUR2019</t>
+  </si>
+  <si>
+    <t>1 USD2012 = 1.113 USD2019</t>
   </si>
 </sst>
 </file>
@@ -857,20 +875,16 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="24" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="43" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="77">
@@ -996,9 +1010,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1036,9 +1050,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1071,26 +1085,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1123,26 +1120,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1316,33 +1296,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1350,141 +1330,171 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="B8" s="11" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75"/>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="6"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B20" s="5"/>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A23" s="5" t="s">
+      <c r="E21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="6"/>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B23" s="5"/>
+      <c r="E23" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A26" s="5" t="s">
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <f>A30*A29</f>
+        <v>1.0057677231492888</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="6"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B26" s="5"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="A29" s="10">
-        <v>0.89290000000000003</v>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f>1/0.8929</f>
+        <v>1.1199462425803561</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" s="9" customFormat="1" x14ac:dyDescent="0.75">
-      <c r="A30" s="9">
+        <v>36</v>
+      </c>
+      <c r="G29" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f>0.89805</f>
         <v>0.89805000000000001</v>
       </c>
-      <c r="B30" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.75">
+      <c r="B30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <f>A29*A30</f>
-        <v>0.801868845</v>
+        <v>1.0057677231492888</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.75">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.75">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.75">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.75">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.75">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.75">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>18</v>
       </c>
@@ -1506,26 +1516,26 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <f>10^9*About!$A$31</f>
-        <v>801868845</v>
+        <v>1005767723.1492888</v>
       </c>
     </row>
   </sheetData>
@@ -1542,23 +1552,23 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="6">
         <f>10^6*About!$A$31</f>
-        <v>801868.84499999997</v>
+        <v>1005767.7231492888</v>
       </c>
     </row>
   </sheetData>
@@ -1573,25 +1583,27 @@
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="31.26953125" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
-      <c r="B1" s="4" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2">
         <f>1*About!A31</f>
-        <v>0.801868845</v>
+        <v>1.0057677231492888</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Currency conversion to 2023 Euros
</commit_message>
<xml_diff>
--- a/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
+++ b/InputData/web-app/OCCF/Output Currency Conversion Factors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\web-app\OCCF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robbie\Dropbox (Energy Innovation)\My Documents\Energy Policy Solutions\European Union\Models\eps-eu\InputData\web-app\OCCF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB702403-E59A-4547-A48B-836A2090D34B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5520020F-DDDE-44C2-B4D0-50CD488CD24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14580" yWindow="1620" windowWidth="26730" windowHeight="20460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Source:</t>
   </si>
@@ -87,47 +87,50 @@
     <t>See cpi.xlsx</t>
   </si>
   <si>
-    <t>value less than 1 in this variable.</t>
-  </si>
-  <si>
-    <t>This is why we multiply, not divide, by the conversion</t>
-  </si>
-  <si>
-    <t>factor above.</t>
-  </si>
-  <si>
     <t>Medium Output Currency Unit</t>
   </si>
   <si>
     <t>OCCF Dollars per Medium Output Currency Unit</t>
   </si>
   <si>
-    <t>Recall, this variable is "dollars per large/medium/small currency output unit"</t>
-  </si>
-  <si>
-    <t>2012 dollars are worth more than 2020 dollars, so we need a</t>
-  </si>
-  <si>
-    <t>2021 dollars per 2012 dollar</t>
-  </si>
-  <si>
-    <t>billion 2021 dollars</t>
-  </si>
-  <si>
-    <t>million 2021 dollars</t>
-  </si>
-  <si>
-    <t>2021 dollars</t>
-  </si>
-  <si>
-    <t>which in this case is "2012 dollars per 2021 dollar."</t>
+    <t>billion 2023 Euros</t>
+  </si>
+  <si>
+    <t>million 2023 Euros</t>
+  </si>
+  <si>
+    <t>2023 Euros</t>
+  </si>
+  <si>
+    <t>2023 Euros per 2012 dollar</t>
+  </si>
+  <si>
+    <t>2023 dollar to 2012 dollar</t>
+  </si>
+  <si>
+    <t>2023 Euro to 2023 dollar</t>
+  </si>
+  <si>
+    <t>https://www.exchangerates.org.uk/EUR-USD-spot-exchange-rates-history-2023.html</t>
+  </si>
+  <si>
+    <t>US Dollar Currency Year Conversion</t>
+  </si>
+  <si>
+    <t>Euro to USD Conversion</t>
+  </si>
+  <si>
+    <t>Exchange Rates UK</t>
+  </si>
+  <si>
+    <t>Average 2023 Rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +146,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +164,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -180,6 +196,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,15 +505,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="A41" sqref="A41:B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -502,7 +523,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -514,119 +535,139 @@
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="9">
+        <v>2024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="5"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B23" s="5"/>
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>0.84730412960844359</v>
-      </c>
-      <c r="B26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="5"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="5"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <f>1/(1/A43/A42)</f>
+        <v>0.81612960000000001</v>
+      </c>
+      <c r="B38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1.0824</v>
+      </c>
+      <c r="B42" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>0.754</v>
+      </c>
+      <c r="B43" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -659,8 +700,8 @@
         <v>8</v>
       </c>
       <c r="B2" s="2">
-        <f>10^9*About!$A$26</f>
-        <v>847304129.60844362</v>
+        <f>10^9*About!$A$38</f>
+        <v>816129600</v>
       </c>
     </row>
   </sheetData>
@@ -692,8 +733,8 @@
         <v>8</v>
       </c>
       <c r="B2" s="6">
-        <f>10^6*About!$A$26</f>
-        <v>847304.12960844359</v>
+        <f>10^6*About!$A$38</f>
+        <v>816129.6</v>
       </c>
     </row>
   </sheetData>
@@ -725,8 +766,8 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <f>1*About!A26</f>
-        <v>0.84730412960844359</v>
+        <f>1*About!A38</f>
+        <v>0.81612960000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>